<commit_message>
add team member names
</commit_message>
<xml_diff>
--- a/use_tot_sector.xlsx
+++ b/use_tot_sector.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\CSEDS\Internet\Data\Consum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c987f5592cee8402/Documents/INST490/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{363F4847-A28A-48DF-91EE-F9C8F5D8D194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" tabRatio="657"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="657" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="7" r:id="rId1"/>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="89">
   <si>
     <t>State</t>
   </si>
@@ -322,11 +323,14 @@
   <si>
     <t>US</t>
   </si>
+  <si>
+    <t>Average retail price (cents/kWh)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -434,7 +438,7 @@
     </xf>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
@@ -449,6 +453,8 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1340,16 +1346,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.8984375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="34.875" style="5" customWidth="1"/>
     <col min="2" max="2" width="43.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.09765625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="14.125" style="5" customWidth="1"/>
     <col min="4" max="4" width="9" style="5"/>
     <col min="5" max="5" width="10" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="5"/>
@@ -1365,12 +1373,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
@@ -1397,7 +1405,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -1414,7 +1422,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -1431,7 +1439,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -1448,7 +1456,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -1465,7 +1473,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -1482,39 +1490,39 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A17" r:id="rId1" display="https://www.eia.gov/state/seds/"/>
-    <hyperlink ref="A19" r:id="rId2" display="SEDS Codes and Descriptions"/>
-    <hyperlink ref="A18" r:id="rId3"/>
-    <hyperlink ref="A10" location="'Residential Sector'!A1" display="Residential Sector"/>
-    <hyperlink ref="A11" location="'Commercial Sector'!A1" display="Commercial Sector"/>
-    <hyperlink ref="A12" location="'Industrial Sector'!A1" display="Industrial Sector"/>
-    <hyperlink ref="A13" location="'Transportation Sector'!A1" display="Transportation Sector"/>
-    <hyperlink ref="A14" location="'Total Consumption'!A1" display="Total Consumption"/>
+    <hyperlink ref="A17" r:id="rId1" display="https://www.eia.gov/state/seds/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A19" r:id="rId2" display="SEDS Codes and Descriptions" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A18" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A10" location="'Residential Sector'!A1" display="Residential Sector" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A11" location="'Commercial Sector'!A1" display="Commercial Sector" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A12" location="'Industrial Sector'!A1" display="Industrial Sector" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A13" location="'Transportation Sector'!A1" display="Transportation Sector" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A14" location="'Total Consumption'!A1" display="Total Consumption" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -1522,32 +1530,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CW55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="BA4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="BO26" sqref="BO26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.09765625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="10.09765625" style="10" customWidth="1"/>
-    <col min="3" max="6" width="10.09765625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="61" width="11.09765625" style="10" bestFit="1" customWidth="1"/>
-    <col min="62" max="16384" width="9" style="10"/>
+    <col min="1" max="1" width="6.125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="10" customWidth="1"/>
+    <col min="3" max="6" width="10.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="61" width="11.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="27.375" style="14" bestFit="1" customWidth="1"/>
+    <col min="63" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:101" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
+      <c r="BJ1" s="14"/>
     </row>
     <row r="2" spans="1:101" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
+      <c r="BJ2" s="14"/>
     </row>
     <row r="3" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -1733,6 +1744,9 @@
       <c r="BI3" s="8">
         <v>2019</v>
       </c>
+      <c r="BJ3" s="14" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="4" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1918,7 +1932,9 @@
       <c r="BI4" s="13">
         <v>48580</v>
       </c>
-      <c r="BJ4" s="11"/>
+      <c r="BJ4" s="15">
+        <v>19.82</v>
+      </c>
       <c r="BK4" s="11"/>
       <c r="BL4" s="11"/>
       <c r="BM4" s="11"/>
@@ -2143,7 +2159,9 @@
       <c r="BI5" s="13">
         <v>347873</v>
       </c>
-      <c r="BJ5" s="11"/>
+      <c r="BJ5" s="15">
+        <v>9.84</v>
+      </c>
       <c r="BK5" s="11"/>
       <c r="BL5" s="11"/>
       <c r="BM5" s="11"/>
@@ -2368,7 +2386,9 @@
       <c r="BI6" s="13">
         <v>226877</v>
       </c>
-      <c r="BJ6" s="11"/>
+      <c r="BJ6" s="14">
+        <v>8.32</v>
+      </c>
       <c r="BK6" s="11"/>
       <c r="BL6" s="11"/>
       <c r="BM6" s="11"/>
@@ -2593,7 +2613,9 @@
       <c r="BI7" s="13">
         <v>412787</v>
       </c>
-      <c r="BJ7" s="11"/>
+      <c r="BJ7" s="15">
+        <v>10.44</v>
+      </c>
       <c r="BK7" s="11"/>
       <c r="BL7" s="11"/>
       <c r="BM7" s="11"/>
@@ -2818,7 +2840,9 @@
       <c r="BI8" s="13">
         <v>1455702</v>
       </c>
-      <c r="BJ8" s="11"/>
+      <c r="BJ8" s="14">
+        <v>18</v>
+      </c>
       <c r="BK8" s="11"/>
       <c r="BL8" s="11"/>
       <c r="BM8" s="11"/>
@@ -3043,7 +3067,9 @@
       <c r="BI9" s="13">
         <v>378983</v>
       </c>
-      <c r="BJ9" s="11"/>
+      <c r="BJ9">
+        <v>10.27</v>
+      </c>
       <c r="BK9" s="11"/>
       <c r="BL9" s="11"/>
       <c r="BM9" s="11"/>
@@ -3268,7 +3294,9 @@
       <c r="BI10" s="13">
         <v>239810</v>
       </c>
-      <c r="BJ10" s="11"/>
+      <c r="BJ10">
+        <v>19.13</v>
+      </c>
       <c r="BK10" s="11"/>
       <c r="BL10" s="11"/>
       <c r="BM10" s="11"/>
@@ -3493,7 +3521,9 @@
       <c r="BI11" s="13">
         <v>39337</v>
       </c>
-      <c r="BJ11" s="11"/>
+      <c r="BJ11">
+        <v>11.9</v>
+      </c>
       <c r="BK11" s="11"/>
       <c r="BL11" s="11"/>
       <c r="BM11" s="11"/>
@@ -3718,7 +3748,9 @@
       <c r="BI12" s="13">
         <v>65584</v>
       </c>
-      <c r="BJ12" s="11"/>
+      <c r="BJ12">
+        <v>10.24</v>
+      </c>
       <c r="BK12" s="11"/>
       <c r="BL12" s="11"/>
       <c r="BM12" s="11"/>
@@ -3943,7 +3975,9 @@
       <c r="BI13" s="13">
         <v>1180439</v>
       </c>
-      <c r="BJ13" s="11"/>
+      <c r="BJ13">
+        <v>10.06</v>
+      </c>
       <c r="BK13" s="11"/>
       <c r="BL13" s="11"/>
       <c r="BM13" s="11"/>
@@ -4168,7 +4202,9 @@
       <c r="BI14" s="13">
         <v>715836</v>
       </c>
-      <c r="BJ14" s="11"/>
+      <c r="BJ14">
+        <v>9.93</v>
+      </c>
       <c r="BK14" s="11"/>
       <c r="BL14" s="11"/>
       <c r="BM14" s="11"/>
@@ -4393,7 +4429,9 @@
       <c r="BI15" s="13">
         <v>34545</v>
       </c>
-      <c r="BJ15" s="11"/>
+      <c r="BJ15">
+        <v>27.55</v>
+      </c>
       <c r="BK15" s="11"/>
       <c r="BL15" s="11"/>
       <c r="BM15" s="11"/>
@@ -4618,7 +4656,9 @@
       <c r="BI16" s="13">
         <v>248336</v>
       </c>
-      <c r="BJ16" s="11"/>
+      <c r="BJ16">
+        <v>8.9700000000000006</v>
+      </c>
       <c r="BK16" s="11"/>
       <c r="BL16" s="11"/>
       <c r="BM16" s="11"/>
@@ -4843,7 +4883,9 @@
       <c r="BI17" s="13">
         <v>136900</v>
       </c>
-      <c r="BJ17" s="11"/>
+      <c r="BJ17">
+        <v>7.99</v>
+      </c>
       <c r="BK17" s="11"/>
       <c r="BL17" s="11"/>
       <c r="BM17" s="11"/>
@@ -5068,7 +5110,9 @@
       <c r="BI18" s="13">
         <v>970625</v>
       </c>
-      <c r="BJ18" s="11"/>
+      <c r="BJ18">
+        <v>9.75</v>
+      </c>
       <c r="BK18" s="11"/>
       <c r="BL18" s="11"/>
       <c r="BM18" s="11"/>
@@ -5293,7 +5337,9 @@
       <c r="BI19" s="13">
         <v>536499</v>
       </c>
-      <c r="BJ19" s="11"/>
+      <c r="BJ19">
+        <v>9.92</v>
+      </c>
       <c r="BK19" s="11"/>
       <c r="BL19" s="11"/>
       <c r="BM19" s="11"/>
@@ -5518,7 +5564,9 @@
       <c r="BI20" s="13">
         <v>228838</v>
       </c>
-      <c r="BJ20" s="11"/>
+      <c r="BJ20">
+        <v>10.38</v>
+      </c>
       <c r="BK20" s="11"/>
       <c r="BL20" s="11"/>
       <c r="BM20" s="11"/>
@@ -5743,7 +5791,9 @@
       <c r="BI21" s="13">
         <v>352177</v>
       </c>
-      <c r="BJ21" s="11"/>
+      <c r="BJ21">
+        <v>8.58</v>
+      </c>
       <c r="BK21" s="11"/>
       <c r="BL21" s="11"/>
       <c r="BM21" s="11"/>
@@ -5968,7 +6018,9 @@
       <c r="BI22" s="13">
         <v>318333</v>
       </c>
-      <c r="BJ22" s="11"/>
+      <c r="BJ22">
+        <v>7.51</v>
+      </c>
       <c r="BK22" s="11"/>
       <c r="BL22" s="11"/>
       <c r="BM22" s="11"/>
@@ -6193,7 +6245,9 @@
       <c r="BI23" s="13">
         <v>432949</v>
       </c>
-      <c r="BJ23" s="11"/>
+      <c r="BJ23">
+        <v>18.190000000000001</v>
+      </c>
       <c r="BK23" s="11"/>
       <c r="BL23" s="11"/>
       <c r="BM23" s="11"/>
@@ -6418,7 +6472,9 @@
       <c r="BI24" s="13">
         <v>393731</v>
       </c>
-      <c r="BJ24" s="11"/>
+      <c r="BJ24">
+        <v>11.15</v>
+      </c>
       <c r="BK24" s="11"/>
       <c r="BL24" s="11"/>
       <c r="BM24" s="11"/>
@@ -6643,7 +6699,9 @@
       <c r="BI25" s="13">
         <v>106253</v>
       </c>
-      <c r="BJ25" s="11"/>
+      <c r="BJ25">
+        <v>13.54</v>
+      </c>
       <c r="BK25" s="11"/>
       <c r="BL25" s="11"/>
       <c r="BM25" s="11"/>
@@ -6868,7 +6926,9 @@
       <c r="BI26" s="13">
         <v>783997</v>
       </c>
-      <c r="BJ26" s="11"/>
+      <c r="BJ26">
+        <v>12.21</v>
+      </c>
       <c r="BK26" s="11"/>
       <c r="BL26" s="11"/>
       <c r="BM26" s="11"/>
@@ -7093,7 +7153,9 @@
       <c r="BI27" s="13">
         <v>418227</v>
       </c>
-      <c r="BJ27" s="11"/>
+      <c r="BJ27">
+        <v>10.57</v>
+      </c>
       <c r="BK27" s="11"/>
       <c r="BL27" s="11"/>
       <c r="BM27" s="11"/>
@@ -7318,7 +7380,9 @@
       <c r="BI28" s="13">
         <v>530235</v>
       </c>
-      <c r="BJ28" s="11"/>
+      <c r="BJ28">
+        <v>9.64</v>
+      </c>
       <c r="BK28" s="11"/>
       <c r="BL28" s="11"/>
       <c r="BM28" s="11"/>
@@ -7543,7 +7607,9 @@
       <c r="BI29" s="13">
         <v>195186</v>
       </c>
-      <c r="BJ29" s="11"/>
+      <c r="BJ29">
+        <v>9.1300000000000008</v>
+      </c>
       <c r="BK29" s="11"/>
       <c r="BL29" s="11"/>
       <c r="BM29" s="11"/>
@@ -7768,7 +7834,9 @@
       <c r="BI30" s="13">
         <v>105697</v>
       </c>
-      <c r="BJ30" s="11"/>
+      <c r="BJ30">
+        <v>9.1300000000000008</v>
+      </c>
       <c r="BK30" s="11"/>
       <c r="BL30" s="11"/>
       <c r="BM30" s="11"/>
@@ -7993,7 +8061,9 @@
       <c r="BI31" s="13">
         <v>696311</v>
       </c>
-      <c r="BJ31" s="11"/>
+      <c r="BJ31">
+        <v>9.43</v>
+      </c>
       <c r="BK31" s="11"/>
       <c r="BL31" s="11"/>
       <c r="BM31" s="11"/>
@@ -8218,7 +8288,9 @@
       <c r="BI32" s="13">
         <v>78903</v>
       </c>
-      <c r="BJ32" s="11"/>
+      <c r="BJ32">
+        <v>8.5299999999999994</v>
+      </c>
       <c r="BK32" s="11"/>
       <c r="BL32" s="11"/>
       <c r="BM32" s="11"/>
@@ -8443,7 +8515,9 @@
       <c r="BI33" s="13">
         <v>169241</v>
       </c>
-      <c r="BJ33" s="11"/>
+      <c r="BJ33">
+        <v>8.9700000000000006</v>
+      </c>
       <c r="BK33" s="11"/>
       <c r="BL33" s="11"/>
       <c r="BM33" s="11"/>
@@ -8668,7 +8742,9 @@
       <c r="BI34" s="13">
         <v>105115</v>
       </c>
-      <c r="BJ34" s="11"/>
+      <c r="BJ34">
+        <v>16.63</v>
+      </c>
       <c r="BK34" s="11"/>
       <c r="BL34" s="11"/>
       <c r="BM34" s="11"/>
@@ -8893,7 +8969,9 @@
       <c r="BI35" s="13">
         <v>563131</v>
       </c>
-      <c r="BJ35" s="11"/>
+      <c r="BJ35">
+        <v>13.63</v>
+      </c>
       <c r="BK35" s="11"/>
       <c r="BL35" s="11"/>
       <c r="BM35" s="11"/>
@@ -9118,7 +9196,9 @@
       <c r="BI36" s="13">
         <v>132449</v>
       </c>
-      <c r="BJ36" s="11"/>
+      <c r="BJ36">
+        <v>9.33</v>
+      </c>
       <c r="BK36" s="11"/>
       <c r="BL36" s="11"/>
       <c r="BM36" s="11"/>
@@ -9343,7 +9423,9 @@
       <c r="BI37" s="13">
         <v>173543</v>
       </c>
-      <c r="BJ37" s="11"/>
+      <c r="BJ37">
+        <v>8.33</v>
+      </c>
       <c r="BK37" s="11"/>
       <c r="BL37" s="11"/>
       <c r="BM37" s="11"/>
@@ -9568,7 +9650,9 @@
       <c r="BI38" s="13">
         <v>1138582</v>
       </c>
-      <c r="BJ38" s="11"/>
+      <c r="BJ38">
+        <v>14.87</v>
+      </c>
       <c r="BK38" s="11"/>
       <c r="BL38" s="11"/>
       <c r="BM38" s="11"/>
@@ -9793,7 +9877,9 @@
       <c r="BI39" s="13">
         <v>875824</v>
       </c>
-      <c r="BJ39" s="11"/>
+      <c r="BJ39">
+        <v>9.44</v>
+      </c>
       <c r="BK39" s="11"/>
       <c r="BL39" s="11"/>
       <c r="BM39" s="11"/>
@@ -10018,7 +10104,9 @@
       <c r="BI40" s="13">
         <v>298943</v>
       </c>
-      <c r="BJ40" s="11"/>
+      <c r="BJ40">
+        <v>7.63</v>
+      </c>
       <c r="BK40" s="11"/>
       <c r="BL40" s="11"/>
       <c r="BM40" s="11"/>
@@ -10243,7 +10331,9 @@
       <c r="BI41" s="13">
         <v>255441</v>
       </c>
-      <c r="BJ41" s="11"/>
+      <c r="BJ41">
+        <v>8.82</v>
+      </c>
       <c r="BK41" s="11"/>
       <c r="BL41" s="11"/>
       <c r="BM41" s="11"/>
@@ -10468,7 +10558,9 @@
       <c r="BI42" s="13">
         <v>891688</v>
       </c>
-      <c r="BJ42" s="11"/>
+      <c r="BJ42">
+        <v>9.6999999999999993</v>
+      </c>
       <c r="BK42" s="11"/>
       <c r="BL42" s="11"/>
       <c r="BM42" s="11"/>
@@ -10693,7 +10785,9 @@
       <c r="BI43" s="13">
         <v>60993</v>
       </c>
-      <c r="BJ43" s="11"/>
+      <c r="BJ43">
+        <v>18.54</v>
+      </c>
       <c r="BK43" s="11"/>
       <c r="BL43" s="11"/>
       <c r="BM43" s="11"/>
@@ -10918,7 +11012,9 @@
       <c r="BI44" s="13">
         <v>365358</v>
       </c>
-      <c r="BJ44" s="11"/>
+      <c r="BJ44">
+        <v>9.9</v>
+      </c>
       <c r="BK44" s="11"/>
       <c r="BL44" s="11"/>
       <c r="BM44" s="11"/>
@@ -11143,7 +11239,9 @@
       <c r="BI45" s="13">
         <v>74163</v>
       </c>
-      <c r="BJ45" s="11"/>
+      <c r="BJ45">
+        <v>10.06</v>
+      </c>
       <c r="BK45" s="11"/>
       <c r="BL45" s="11"/>
       <c r="BM45" s="11"/>
@@ -11368,7 +11466,9 @@
       <c r="BI46" s="13">
         <v>524772</v>
       </c>
-      <c r="BJ46" s="11"/>
+      <c r="BJ46">
+        <v>9.52</v>
+      </c>
       <c r="BK46" s="11"/>
       <c r="BL46" s="11"/>
       <c r="BM46" s="11"/>
@@ -11593,7 +11693,9 @@
       <c r="BI47" s="13">
         <v>1767320</v>
       </c>
-      <c r="BJ47" s="11"/>
+      <c r="BJ47">
+        <v>8.36</v>
+      </c>
       <c r="BK47" s="11"/>
       <c r="BL47" s="11"/>
       <c r="BM47" s="11"/>
@@ -11818,7 +11920,9 @@
       <c r="BI48" s="13">
         <v>187767</v>
       </c>
-      <c r="BJ48" s="11"/>
+      <c r="BJ48">
+        <v>8.27</v>
+      </c>
       <c r="BK48" s="11"/>
       <c r="BL48" s="11"/>
       <c r="BM48" s="11"/>
@@ -12043,7 +12147,9 @@
       <c r="BI49" s="13">
         <v>571741</v>
       </c>
-      <c r="BJ49" s="11"/>
+      <c r="BJ49">
+        <v>16.329999999999998</v>
+      </c>
       <c r="BK49" s="11"/>
       <c r="BL49" s="11"/>
       <c r="BM49" s="11"/>
@@ -12268,7 +12374,9 @@
       <c r="BI50" s="13">
         <v>47847</v>
       </c>
-      <c r="BJ50" s="11"/>
+      <c r="BJ50">
+        <v>9.16</v>
+      </c>
       <c r="BK50" s="11"/>
       <c r="BL50" s="11"/>
       <c r="BM50" s="11"/>
@@ -12493,7 +12601,9 @@
       <c r="BI51" s="13">
         <v>496532</v>
       </c>
-      <c r="BJ51" s="11"/>
+      <c r="BJ51">
+        <v>8.33</v>
+      </c>
       <c r="BK51" s="11"/>
       <c r="BL51" s="11"/>
       <c r="BM51" s="11"/>
@@ -12718,7 +12828,9 @@
       <c r="BI52" s="13">
         <v>447185</v>
       </c>
-      <c r="BJ52" s="11"/>
+      <c r="BJ52">
+        <v>10.82</v>
+      </c>
       <c r="BK52" s="11"/>
       <c r="BL52" s="11"/>
       <c r="BM52" s="11"/>
@@ -12943,7 +13055,9 @@
       <c r="BI53" s="13">
         <v>156114</v>
       </c>
-      <c r="BJ53" s="11"/>
+      <c r="BJ53">
+        <v>8.75</v>
+      </c>
       <c r="BK53" s="11"/>
       <c r="BL53" s="11"/>
       <c r="BM53" s="11"/>
@@ -13168,7 +13282,9 @@
       <c r="BI54" s="13">
         <v>53913</v>
       </c>
-      <c r="BJ54" s="11"/>
+      <c r="BJ54">
+        <v>8.27</v>
+      </c>
       <c r="BK54" s="11"/>
       <c r="BL54" s="11"/>
       <c r="BM54" s="11"/>
@@ -13393,7 +13509,9 @@
       <c r="BI55" s="13">
         <v>21037214</v>
       </c>
-      <c r="BJ55" s="11"/>
+      <c r="BJ55">
+        <v>10.59</v>
+      </c>
       <c r="BK55" s="11"/>
       <c r="BL55" s="11"/>
       <c r="BM55" s="11"/>
@@ -13441,24 +13559,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CW55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AZ4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="BH1" sqref="BH1:BH1048576"/>
       <selection pane="topRight" activeCell="BH1" sqref="BH1:BH1048576"/>
       <selection pane="bottomLeft" activeCell="BH1" sqref="BH1:BH1048576"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="BJ3" sqref="BJ3:BJ55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.09765625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="10.09765625" style="10" customWidth="1"/>
-    <col min="3" max="6" width="10.09765625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="61" width="11.09765625" style="10" bestFit="1" customWidth="1"/>
-    <col min="62" max="16384" width="9" style="10"/>
+    <col min="1" max="1" width="6.125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="10" customWidth="1"/>
+    <col min="3" max="6" width="10.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="61" width="11.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="27.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="63" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:101" customFormat="1" x14ac:dyDescent="0.25">
@@ -13653,6 +13772,9 @@
       <c r="BI3" s="8">
         <v>2019</v>
       </c>
+      <c r="BJ3" s="14" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="4" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -13838,7 +13960,9 @@
       <c r="BI4" s="13">
         <v>56959</v>
       </c>
-      <c r="BJ4" s="11"/>
+      <c r="BJ4" s="15">
+        <v>19.82</v>
+      </c>
       <c r="BK4" s="11"/>
       <c r="BL4" s="11"/>
       <c r="BM4" s="11"/>
@@ -14063,7 +14187,9 @@
       <c r="BI5" s="13">
         <v>257727</v>
       </c>
-      <c r="BJ5" s="11"/>
+      <c r="BJ5" s="15">
+        <v>9.84</v>
+      </c>
       <c r="BK5" s="11"/>
       <c r="BL5" s="11"/>
       <c r="BM5" s="11"/>
@@ -14288,7 +14414,9 @@
       <c r="BI6" s="13">
         <v>180162</v>
       </c>
-      <c r="BJ6" s="11"/>
+      <c r="BJ6" s="14">
+        <v>8.32</v>
+      </c>
       <c r="BK6" s="11"/>
       <c r="BL6" s="11"/>
       <c r="BM6" s="11"/>
@@ -14513,7 +14641,9 @@
       <c r="BI7" s="13">
         <v>347401</v>
       </c>
-      <c r="BJ7" s="11"/>
+      <c r="BJ7" s="15">
+        <v>10.44</v>
+      </c>
       <c r="BK7" s="11"/>
       <c r="BL7" s="11"/>
       <c r="BM7" s="11"/>
@@ -14738,7 +14868,9 @@
       <c r="BI8" s="13">
         <v>1468088</v>
       </c>
-      <c r="BJ8" s="11"/>
+      <c r="BJ8" s="14">
+        <v>18</v>
+      </c>
       <c r="BK8" s="11"/>
       <c r="BL8" s="11"/>
       <c r="BM8" s="11"/>
@@ -14963,7 +15095,9 @@
       <c r="BI9" s="13">
         <v>300962</v>
       </c>
-      <c r="BJ9" s="11"/>
+      <c r="BJ9">
+        <v>10.27</v>
+      </c>
       <c r="BK9" s="11"/>
       <c r="BL9" s="11"/>
       <c r="BM9" s="11"/>
@@ -15188,7 +15322,9 @@
       <c r="BI10" s="13">
         <v>187749</v>
       </c>
-      <c r="BJ10" s="11"/>
+      <c r="BJ10">
+        <v>19.13</v>
+      </c>
       <c r="BK10" s="11"/>
       <c r="BL10" s="11"/>
       <c r="BM10" s="11"/>
@@ -15413,7 +15549,9 @@
       <c r="BI11" s="13">
         <v>101339</v>
       </c>
-      <c r="BJ11" s="11"/>
+      <c r="BJ11">
+        <v>11.9</v>
+      </c>
       <c r="BK11" s="11"/>
       <c r="BL11" s="11"/>
       <c r="BM11" s="11"/>
@@ -15638,7 +15776,9 @@
       <c r="BI12" s="13">
         <v>61047</v>
       </c>
-      <c r="BJ12" s="11"/>
+      <c r="BJ12">
+        <v>10.24</v>
+      </c>
       <c r="BK12" s="11"/>
       <c r="BL12" s="11"/>
       <c r="BM12" s="11"/>
@@ -15863,7 +16003,9 @@
       <c r="BI13" s="13">
         <v>966489</v>
       </c>
-      <c r="BJ13" s="11"/>
+      <c r="BJ13">
+        <v>10.06</v>
+      </c>
       <c r="BK13" s="11"/>
       <c r="BL13" s="11"/>
       <c r="BM13" s="11"/>
@@ -16088,7 +16230,9 @@
       <c r="BI14" s="13">
         <v>539326</v>
       </c>
-      <c r="BJ14" s="11"/>
+      <c r="BJ14">
+        <v>9.93</v>
+      </c>
       <c r="BK14" s="11"/>
       <c r="BL14" s="11"/>
       <c r="BM14" s="11"/>
@@ -16313,7 +16457,9 @@
       <c r="BI15" s="13">
         <v>42895</v>
       </c>
-      <c r="BJ15" s="11"/>
+      <c r="BJ15">
+        <v>27.55</v>
+      </c>
       <c r="BK15" s="11"/>
       <c r="BL15" s="11"/>
       <c r="BM15" s="11"/>
@@ -16538,7 +16684,9 @@
       <c r="BI16" s="13">
         <v>201061</v>
       </c>
-      <c r="BJ16" s="11"/>
+      <c r="BJ16">
+        <v>8.9700000000000006</v>
+      </c>
       <c r="BK16" s="11"/>
       <c r="BL16" s="11"/>
       <c r="BM16" s="11"/>
@@ -16763,7 +16911,9 @@
       <c r="BI17" s="13">
         <v>92502</v>
       </c>
-      <c r="BJ17" s="11"/>
+      <c r="BJ17">
+        <v>7.99</v>
+      </c>
       <c r="BK17" s="11"/>
       <c r="BL17" s="11"/>
       <c r="BM17" s="11"/>
@@ -16988,7 +17138,9 @@
       <c r="BI18" s="13">
         <v>808854</v>
       </c>
-      <c r="BJ18" s="11"/>
+      <c r="BJ18">
+        <v>9.75</v>
+      </c>
       <c r="BK18" s="11"/>
       <c r="BL18" s="11"/>
       <c r="BM18" s="11"/>
@@ -17213,7 +17365,9 @@
       <c r="BI19" s="13">
         <v>366790</v>
       </c>
-      <c r="BJ19" s="11"/>
+      <c r="BJ19">
+        <v>9.92</v>
+      </c>
       <c r="BK19" s="11"/>
       <c r="BL19" s="11"/>
       <c r="BM19" s="11"/>
@@ -17438,7 +17592,9 @@
       <c r="BI20" s="13">
         <v>218734</v>
       </c>
-      <c r="BJ20" s="11"/>
+      <c r="BJ20">
+        <v>10.38</v>
+      </c>
       <c r="BK20" s="11"/>
       <c r="BL20" s="11"/>
       <c r="BM20" s="11"/>
@@ -17663,7 +17819,9 @@
       <c r="BI21" s="13">
         <v>260106</v>
       </c>
-      <c r="BJ21" s="11"/>
+      <c r="BJ21">
+        <v>8.58</v>
+      </c>
       <c r="BK21" s="11"/>
       <c r="BL21" s="11"/>
       <c r="BM21" s="11"/>
@@ -17888,7 +18046,9 @@
       <c r="BI22" s="13">
         <v>259841</v>
       </c>
-      <c r="BJ22" s="11"/>
+      <c r="BJ22">
+        <v>7.51</v>
+      </c>
       <c r="BK22" s="11"/>
       <c r="BL22" s="11"/>
       <c r="BM22" s="11"/>
@@ -18113,7 +18273,9 @@
       <c r="BI23" s="13">
         <v>409658</v>
       </c>
-      <c r="BJ23" s="11"/>
+      <c r="BJ23">
+        <v>18.190000000000001</v>
+      </c>
       <c r="BK23" s="11"/>
       <c r="BL23" s="11"/>
       <c r="BM23" s="11"/>
@@ -18338,7 +18500,9 @@
       <c r="BI24" s="13">
         <v>396546</v>
       </c>
-      <c r="BJ24" s="11"/>
+      <c r="BJ24">
+        <v>11.15</v>
+      </c>
       <c r="BK24" s="11"/>
       <c r="BL24" s="11"/>
       <c r="BM24" s="11"/>
@@ -18563,7 +18727,9 @@
       <c r="BI25" s="13">
         <v>67625</v>
       </c>
-      <c r="BJ25" s="11"/>
+      <c r="BJ25">
+        <v>13.54</v>
+      </c>
       <c r="BK25" s="11"/>
       <c r="BL25" s="11"/>
       <c r="BM25" s="11"/>
@@ -18788,7 +18954,9 @@
       <c r="BI26" s="13">
         <v>612415</v>
       </c>
-      <c r="BJ26" s="11"/>
+      <c r="BJ26">
+        <v>12.21</v>
+      </c>
       <c r="BK26" s="11"/>
       <c r="BL26" s="11"/>
       <c r="BM26" s="11"/>
@@ -19013,7 +19181,9 @@
       <c r="BI27" s="13">
         <v>356842</v>
       </c>
-      <c r="BJ27" s="11"/>
+      <c r="BJ27">
+        <v>10.57</v>
+      </c>
       <c r="BK27" s="11"/>
       <c r="BL27" s="11"/>
       <c r="BM27" s="11"/>
@@ -19238,7 +19408,9 @@
       <c r="BI28" s="13">
         <v>407111</v>
       </c>
-      <c r="BJ28" s="11"/>
+      <c r="BJ28">
+        <v>9.64</v>
+      </c>
       <c r="BK28" s="11"/>
       <c r="BL28" s="11"/>
       <c r="BM28" s="11"/>
@@ -19463,7 +19635,9 @@
       <c r="BI29" s="13">
         <v>154067</v>
       </c>
-      <c r="BJ29" s="11"/>
+      <c r="BJ29">
+        <v>9.1300000000000008</v>
+      </c>
       <c r="BK29" s="11"/>
       <c r="BL29" s="11"/>
       <c r="BM29" s="11"/>
@@ -19688,7 +19862,9 @@
       <c r="BI30" s="13">
         <v>87001</v>
       </c>
-      <c r="BJ30" s="11"/>
+      <c r="BJ30">
+        <v>9.1300000000000008</v>
+      </c>
       <c r="BK30" s="11"/>
       <c r="BL30" s="11"/>
       <c r="BM30" s="11"/>
@@ -19913,7 +20089,9 @@
       <c r="BI31" s="13">
         <v>577815</v>
       </c>
-      <c r="BJ31" s="11"/>
+      <c r="BJ31">
+        <v>9.43</v>
+      </c>
       <c r="BK31" s="11"/>
       <c r="BL31" s="11"/>
       <c r="BM31" s="11"/>
@@ -20138,7 +20316,9 @@
       <c r="BI32" s="13">
         <v>97206</v>
       </c>
-      <c r="BJ32" s="11"/>
+      <c r="BJ32">
+        <v>8.5299999999999994</v>
+      </c>
       <c r="BK32" s="11"/>
       <c r="BL32" s="11"/>
       <c r="BM32" s="11"/>
@@ -20363,7 +20543,9 @@
       <c r="BI33" s="13">
         <v>148329</v>
       </c>
-      <c r="BJ33" s="11"/>
+      <c r="BJ33">
+        <v>8.9700000000000006</v>
+      </c>
       <c r="BK33" s="11"/>
       <c r="BL33" s="11"/>
       <c r="BM33" s="11"/>
@@ -20588,7 +20770,9 @@
       <c r="BI34" s="13">
         <v>71036</v>
       </c>
-      <c r="BJ34" s="11"/>
+      <c r="BJ34">
+        <v>16.63</v>
+      </c>
       <c r="BK34" s="11"/>
       <c r="BL34" s="11"/>
       <c r="BM34" s="11"/>
@@ -20813,7 +20997,9 @@
       <c r="BI35" s="13">
         <v>557469</v>
       </c>
-      <c r="BJ35" s="11"/>
+      <c r="BJ35">
+        <v>13.63</v>
+      </c>
       <c r="BK35" s="11"/>
       <c r="BL35" s="11"/>
       <c r="BM35" s="11"/>
@@ -21038,7 +21224,9 @@
       <c r="BI36" s="13">
         <v>129204</v>
       </c>
-      <c r="BJ36" s="11"/>
+      <c r="BJ36">
+        <v>9.33</v>
+      </c>
       <c r="BK36" s="11"/>
       <c r="BL36" s="11"/>
       <c r="BM36" s="11"/>
@@ -21263,7 +21451,9 @@
       <c r="BI37" s="13">
         <v>153879</v>
       </c>
-      <c r="BJ37" s="11"/>
+      <c r="BJ37">
+        <v>8.33</v>
+      </c>
       <c r="BK37" s="11"/>
       <c r="BL37" s="11"/>
       <c r="BM37" s="11"/>
@@ -21488,7 +21678,9 @@
       <c r="BI38" s="13">
         <v>1122017</v>
       </c>
-      <c r="BJ38" s="11"/>
+      <c r="BJ38">
+        <v>14.87</v>
+      </c>
       <c r="BK38" s="11"/>
       <c r="BL38" s="11"/>
       <c r="BM38" s="11"/>
@@ -21713,7 +21905,9 @@
       <c r="BI39" s="13">
         <v>678292</v>
       </c>
-      <c r="BJ39" s="11"/>
+      <c r="BJ39">
+        <v>9.44</v>
+      </c>
       <c r="BK39" s="11"/>
       <c r="BL39" s="11"/>
       <c r="BM39" s="11"/>
@@ -21938,7 +22132,9 @@
       <c r="BI40" s="13">
         <v>244838</v>
       </c>
-      <c r="BJ40" s="11"/>
+      <c r="BJ40">
+        <v>7.63</v>
+      </c>
       <c r="BK40" s="11"/>
       <c r="BL40" s="11"/>
       <c r="BM40" s="11"/>
@@ -22163,7 +22359,9 @@
       <c r="BI41" s="13">
         <v>195845</v>
       </c>
-      <c r="BJ41" s="11"/>
+      <c r="BJ41">
+        <v>8.82</v>
+      </c>
       <c r="BK41" s="11"/>
       <c r="BL41" s="11"/>
       <c r="BM41" s="11"/>
@@ -22388,7 +22586,9 @@
       <c r="BI42" s="13">
         <v>601459</v>
       </c>
-      <c r="BJ42" s="11"/>
+      <c r="BJ42">
+        <v>9.6999999999999993</v>
+      </c>
       <c r="BK42" s="11"/>
       <c r="BL42" s="11"/>
       <c r="BM42" s="11"/>
@@ -22613,7 +22813,9 @@
       <c r="BI43" s="13">
         <v>48052</v>
       </c>
-      <c r="BJ43" s="11"/>
+      <c r="BJ43">
+        <v>18.54</v>
+      </c>
       <c r="BK43" s="11"/>
       <c r="BL43" s="11"/>
       <c r="BM43" s="11"/>
@@ -22838,7 +23040,9 @@
       <c r="BI44" s="13">
         <v>271618</v>
       </c>
-      <c r="BJ44" s="11"/>
+      <c r="BJ44">
+        <v>9.9</v>
+      </c>
       <c r="BK44" s="11"/>
       <c r="BL44" s="11"/>
       <c r="BM44" s="11"/>
@@ -23063,7 +23267,9 @@
       <c r="BI45" s="13">
         <v>65449</v>
       </c>
-      <c r="BJ45" s="11"/>
+      <c r="BJ45">
+        <v>10.06</v>
+      </c>
       <c r="BK45" s="11"/>
       <c r="BL45" s="11"/>
       <c r="BM45" s="11"/>
@@ -23288,7 +23494,9 @@
       <c r="BI46" s="13">
         <v>447089</v>
       </c>
-      <c r="BJ46" s="11"/>
+      <c r="BJ46">
+        <v>9.52</v>
+      </c>
       <c r="BK46" s="11"/>
       <c r="BL46" s="11"/>
       <c r="BM46" s="11"/>
@@ -23513,7 +23721,9 @@
       <c r="BI47" s="13">
         <v>1626670</v>
       </c>
-      <c r="BJ47" s="11"/>
+      <c r="BJ47">
+        <v>8.36</v>
+      </c>
       <c r="BK47" s="11"/>
       <c r="BL47" s="11"/>
       <c r="BM47" s="11"/>
@@ -23738,7 +23948,9 @@
       <c r="BI48" s="13">
         <v>176564</v>
       </c>
-      <c r="BJ48" s="11"/>
+      <c r="BJ48">
+        <v>8.27</v>
+      </c>
       <c r="BK48" s="11"/>
       <c r="BL48" s="11"/>
       <c r="BM48" s="11"/>
@@ -23963,7 +24175,9 @@
       <c r="BI49" s="13">
         <v>631160</v>
       </c>
-      <c r="BJ49" s="11"/>
+      <c r="BJ49">
+        <v>16.329999999999998</v>
+      </c>
       <c r="BK49" s="11"/>
       <c r="BL49" s="11"/>
       <c r="BM49" s="11"/>
@@ -24188,7 +24402,9 @@
       <c r="BI50" s="13">
         <v>25937</v>
       </c>
-      <c r="BJ50" s="11"/>
+      <c r="BJ50">
+        <v>9.16</v>
+      </c>
       <c r="BK50" s="11"/>
       <c r="BL50" s="11"/>
       <c r="BM50" s="11"/>
@@ -24413,7 +24629,9 @@
       <c r="BI51" s="13">
         <v>370191</v>
       </c>
-      <c r="BJ51" s="11"/>
+      <c r="BJ51">
+        <v>8.33</v>
+      </c>
       <c r="BK51" s="11"/>
       <c r="BL51" s="11"/>
       <c r="BM51" s="11"/>
@@ -24638,7 +24856,9 @@
       <c r="BI52" s="13">
         <v>362969</v>
       </c>
-      <c r="BJ52" s="11"/>
+      <c r="BJ52">
+        <v>10.82</v>
+      </c>
       <c r="BK52" s="11"/>
       <c r="BL52" s="11"/>
       <c r="BM52" s="11"/>
@@ -24863,7 +25083,9 @@
       <c r="BI53" s="13">
         <v>111765</v>
       </c>
-      <c r="BJ53" s="11"/>
+      <c r="BJ53">
+        <v>8.75</v>
+      </c>
       <c r="BK53" s="11"/>
       <c r="BL53" s="11"/>
       <c r="BM53" s="11"/>
@@ -25088,7 +25310,9 @@
       <c r="BI54" s="13">
         <v>57342</v>
       </c>
-      <c r="BJ54" s="11"/>
+      <c r="BJ54">
+        <v>8.27</v>
+      </c>
       <c r="BK54" s="11"/>
       <c r="BL54" s="11"/>
       <c r="BM54" s="11"/>
@@ -25313,7 +25537,9 @@
       <c r="BI55" s="13">
         <v>17981489</v>
       </c>
-      <c r="BJ55" s="11"/>
+      <c r="BJ55">
+        <v>10.59</v>
+      </c>
       <c r="BK55" s="11"/>
       <c r="BL55" s="11"/>
       <c r="BM55" s="11"/>
@@ -25360,7 +25586,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:CW55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25371,12 +25597,12 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.09765625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="10.09765625" style="10" customWidth="1"/>
-    <col min="3" max="6" width="10.09765625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="61" width="11.09765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="10" customWidth="1"/>
+    <col min="3" max="6" width="10.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="61" width="11.125" style="10" bestFit="1" customWidth="1"/>
     <col min="62" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
@@ -37279,7 +37505,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:CW55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -37289,12 +37515,12 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.09765625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="10.09765625" style="10" customWidth="1"/>
-    <col min="3" max="6" width="10.09765625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="61" width="11.09765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="10" customWidth="1"/>
+    <col min="3" max="6" width="10.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="61" width="11.125" style="10" bestFit="1" customWidth="1"/>
     <col min="62" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
@@ -49197,7 +49423,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:CW55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -49207,12 +49433,12 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.09765625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="10.09765625" style="10" customWidth="1"/>
-    <col min="3" max="6" width="10.09765625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="61" width="11.09765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="10" customWidth="1"/>
+    <col min="3" max="6" width="10.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="61" width="11.125" style="10" bestFit="1" customWidth="1"/>
     <col min="62" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
move table of contents to sidebar
</commit_message>
<xml_diff>
--- a/use_tot_sector.xlsx
+++ b/use_tot_sector.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UMD\2022 Spring\INST490\INST490-Capstone-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C99FB14-C77B-42FC-9319-C43FE3E09C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B490FC-91F3-4F7F-888F-294C9D27E207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2622" yWindow="2226" windowWidth="17280" windowHeight="8904" tabRatio="657" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="564" yWindow="1938" windowWidth="17280" windowHeight="8904" tabRatio="657" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="7" r:id="rId1"/>

</xml_diff>